<commit_message>
Successful test of exe
</commit_message>
<xml_diff>
--- a/input_template.xlsx
+++ b/input_template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JJ/Dropbox/Work-Personal Sync/Falsification/Scripts/Sourced/facial recognition/Facial-Validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jjacobson\Documents\Dropbox\Work-Personal Sync\Falsification\Scripts\Sourced\facial recognition\Facial-Validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>File Pairings Path</t>
   </si>
@@ -35,18 +35,32 @@
     <t>Images Path</t>
   </si>
   <si>
-    <t>/Users/JJ/Dropbox/Work-Personal Sync/Falsification/Scripts/Sourced/facial recognition/Facial-Validation/demo_faces/demo_filename_pairings.xlsx</t>
-  </si>
-  <si>
-    <t>/Users/JJ/Dropbox/Work-Personal Sync/Falsification/Scripts/Sourced/facial recognition/Facial-Validation/demo_faces/</t>
+    <t>File Needed</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>C:\Users\Jjacobson\Documents\Dropbox\Work-Personal Sync\Falsification\Scripts\Sourced\facial recognition\Facial-Validation\demo_faces\demo_filename_pairings.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\Jjacobson\Documents\Dropbox\Work-Personal Sync\Falsification\Scripts\Sourced\facial recognition\Facial-Validation\demo_faces\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -74,8 +88,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -85,6 +102,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -353,34 +373,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="124.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Since sheet template, filter warnings, removed excess code, csv template
</commit_message>
<xml_diff>
--- a/input_template.xlsx
+++ b/input_template.xlsx
@@ -27,31 +27,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
-  <si>
-    <t>File Pairings Path</t>
-  </si>
-  <si>
-    <t>Images Path</t>
-  </si>
-  <si>
-    <t>File Needed</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>C:\Users\Jjacobson\Documents\Dropbox\Work-Personal Sync\Falsification\Scripts\Sourced\facial recognition\Facial-Validation\demo_faces\demo_filename_pairings.xlsx</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>C:\Users\Jjacobson\Documents\Dropbox\Work-Personal Sync\Falsification\Scripts\Sourced\facial recognition\Facial-Validation\demo_faces\</t>
+  </si>
+  <si>
+    <t>Image 1</t>
+  </si>
+  <si>
+    <t>Image 2</t>
+  </si>
+  <si>
+    <t>kyi1.jpg</t>
+  </si>
+  <si>
+    <t>freeman1.jpg</t>
+  </si>
+  <si>
+    <t>kyi2.jpg</t>
+  </si>
+  <si>
+    <t>thida1.jpg</t>
+  </si>
+  <si>
+    <t>mandela+others.jpg</t>
+  </si>
+  <si>
+    <t>mandela2.jpg</t>
+  </si>
+  <si>
+    <t>mandela1.jpg</t>
+  </si>
+  <si>
+    <t>mandela3.jpg</t>
+  </si>
+  <si>
+    <t>mobama1.jpg</t>
+  </si>
+  <si>
+    <t>mobama2.jpg</t>
+  </si>
+  <si>
+    <t>bobama2.jpg</t>
+  </si>
+  <si>
+    <t>bobama5.jpg</t>
+  </si>
+  <si>
+    <t>bobama3.jpg</t>
+  </si>
+  <si>
+    <t>Image Directory</t>
+  </si>
+  <si>
+    <t>Directory Needed</t>
+  </si>
+  <si>
+    <t>Path of Directory (i.e. C:\faces\)</t>
+  </si>
+  <si>
+    <t>Input the directory containing images, and the names of the image files, where indicated. The directory path must be in cell B2, while the image filenames must begin in row 5 and be in columns A and B. The list of images can be as long as desired.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -67,6 +109,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -76,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -84,14 +140,123 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -373,48 +538,228 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="124.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.25" customWidth="1"/>
+    <col min="2" max="2" width="28.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="9"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="9"/>
+    </row>
+    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C4:K14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>